<commit_message>
adding rows and updating dummy data in booking sheet
</commit_message>
<xml_diff>
--- a/src/data/cSpace_booking.xlsx
+++ b/src/data/cSpace_booking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="2018-07" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="73">
   <si>
     <t xml:space="preserve">First Floor Hall</t>
   </si>
@@ -128,6 +128,12 @@
     <t xml:space="preserve">Carri Cordon</t>
   </si>
   <si>
+    <t xml:space="preserve">carri@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123-456-7890</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caren Alsop</t>
   </si>
   <si>
@@ -138,6 +144,12 @@
   </si>
   <si>
     <t xml:space="preserve">Delcie Montalvan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delcie@cspace.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">987-654-3210</t>
   </si>
   <si>
     <t xml:space="preserve">Doesn't pay</t>
@@ -360,7 +372,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="T21:T23 H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -855,7 +867,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="T21:T23 H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1392,7 +1404,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="T21:T23 H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1965,7 +1977,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U22" activeCellId="1" sqref="T21:T23 U22"/>
+      <selection pane="topLeft" activeCell="U22" activeCellId="0" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2573,8 +2585,8 @@
   </sheetPr>
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T21" activeCellId="0" sqref="T21:T23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T21" activeCellId="0" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3182,15 +3194,15 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="T21:T23 A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.44"/>
@@ -3220,125 +3232,141 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="carri@example.com"/>
+    <hyperlink ref="B5" r:id="rId2" display="delcie@cspace.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3357,7 +3385,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="T21:T23 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3372,16 +3400,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
@@ -3392,10 +3420,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3403,10 +3431,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,10 +3442,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3425,10 +3453,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3436,10 +3464,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,10 +3475,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,10 +3486,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3469,10 +3497,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3480,10 +3508,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,10 +3519,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3502,10 +3530,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3513,10 +3541,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3524,10 +3552,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3535,10 +3563,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,10 +3574,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3557,10 +3585,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3568,10 +3596,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3579,10 +3607,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3604,7 +3632,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="T21:T23 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3615,21 +3643,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -3637,10 +3665,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>5</v>
@@ -3648,10 +3676,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
@@ -3659,10 +3687,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>20</v>
@@ -3670,10 +3698,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>20</v>

</xml_diff>